<commit_message>
borre a Adriana Mendoza dupl y deje solo la torta
</commit_message>
<xml_diff>
--- a/data_limpia.xlsx
+++ b/data_limpia.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manue\Desktop\bot_cumple_weplan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manue\Desktop\Developer\Proyectos\birthday_greeting_bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D366AE36-B3C3-442F-8709-DBBFE6FCA7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7E5274-4832-43FD-96F6-A624DC8CC6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$D$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$55</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
   <si>
     <t>nombre</t>
   </si>
@@ -230,12 +230,6 @@
   </si>
   <si>
     <t>andres.gerola@solar-insights.com</t>
-  </si>
-  <si>
-    <t>Adriana Mendoza</t>
-  </si>
-  <si>
-    <t>adriana.mendoza@solar-insights.com</t>
   </si>
   <si>
     <t>Matias Bedacarratz</t>
@@ -680,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L997"/>
+  <dimension ref="A1:L996"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1237,13 +1231,13 @@
     </row>
     <row r="34" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C34" s="5">
-        <v>25303</v>
+        <v>302</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>68</v>
@@ -1253,13 +1247,13 @@
     </row>
     <row r="35" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>69</v>
       </c>
       <c r="C35" s="5">
-        <v>302</v>
+        <v>23725</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>70</v>
@@ -1269,13 +1263,13 @@
     </row>
     <row r="36" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C36" s="5">
-        <v>23725</v>
+        <v>25303</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>72</v>
@@ -1291,7 +1285,7 @@
         <v>73</v>
       </c>
       <c r="C37" s="5">
-        <v>25303</v>
+        <v>34205</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>74</v>
@@ -1307,7 +1301,7 @@
         <v>75</v>
       </c>
       <c r="C38" s="5">
-        <v>34205</v>
+        <v>30215</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>76</v>
@@ -1323,7 +1317,7 @@
         <v>77</v>
       </c>
       <c r="C39" s="5">
-        <v>30215</v>
+        <v>36879</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>78</v>
@@ -1339,7 +1333,7 @@
         <v>79</v>
       </c>
       <c r="C40" s="5">
-        <v>36879</v>
+        <v>35873</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>80</v>
@@ -1355,7 +1349,7 @@
         <v>81</v>
       </c>
       <c r="C41" s="5">
-        <v>35873</v>
+        <v>36662</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>82</v>
@@ -1371,7 +1365,7 @@
         <v>83</v>
       </c>
       <c r="C42" s="5">
-        <v>36662</v>
+        <v>37687</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>84</v>
@@ -1387,7 +1381,7 @@
         <v>85</v>
       </c>
       <c r="C43" s="5">
-        <v>37687</v>
+        <v>35398</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>86</v>
@@ -1403,7 +1397,7 @@
         <v>87</v>
       </c>
       <c r="C44" s="5">
-        <v>35398</v>
+        <v>35952</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>88</v>
@@ -1419,7 +1413,7 @@
         <v>89</v>
       </c>
       <c r="C45" s="5">
-        <v>35952</v>
+        <v>35735</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>90</v>
@@ -1435,7 +1429,7 @@
         <v>91</v>
       </c>
       <c r="C46" s="5">
-        <v>35735</v>
+        <v>37126</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>92</v>
@@ -1451,7 +1445,7 @@
         <v>93</v>
       </c>
       <c r="C47" s="5">
-        <v>37126</v>
+        <v>34110</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>94</v>
@@ -1467,7 +1461,7 @@
         <v>95</v>
       </c>
       <c r="C48" s="5">
-        <v>34110</v>
+        <v>36765</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>96</v>
@@ -1483,7 +1477,7 @@
         <v>97</v>
       </c>
       <c r="C49" s="5">
-        <v>36765</v>
+        <v>37181</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>98</v>
@@ -1499,7 +1493,7 @@
         <v>99</v>
       </c>
       <c r="C50" s="5">
-        <v>37181</v>
+        <v>35736</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>100</v>
@@ -1512,13 +1506,13 @@
         <v>52</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C51" s="5">
+        <v>31012</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="C51" s="5">
-        <v>35736</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="F51" s="4"/>
       <c r="L51" s="4"/>
@@ -1528,13 +1522,13 @@
         <v>53</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C52" s="5">
-        <v>31012</v>
+        <v>34536</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F52" s="4"/>
       <c r="L52" s="4"/>
@@ -1544,10 +1538,10 @@
         <v>54</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C53" s="5">
-        <v>34536</v>
+        <v>36988</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>104</v>
@@ -1560,13 +1554,13 @@
         <v>55</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C54" s="5">
+        <v>28401</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="C54" s="5">
-        <v>36988</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="F54" s="4"/>
       <c r="L54" s="4"/>
@@ -1575,31 +1569,23 @@
       <c r="A55" s="2">
         <v>56</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>111</v>
+      <c r="B55" s="7" t="s">
+        <v>110</v>
       </c>
       <c r="C55" s="5">
-        <v>28401</v>
+        <v>24941</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F55" s="4"/>
       <c r="L55" s="4"/>
     </row>
     <row r="56" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="2">
-        <v>57</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C56" s="5">
-        <v>24941</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>108</v>
-      </c>
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="1"/>
       <c r="F56" s="4"/>
       <c r="L56" s="4"/>
     </row>
@@ -9123,32 +9109,24 @@
       <c r="F996" s="4"/>
       <c r="L996" s="4"/>
     </row>
-    <row r="997" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A997" s="1"/>
-      <c r="B997" s="1"/>
-      <c r="C997" s="5"/>
-      <c r="D997" s="1"/>
-      <c r="F997" s="4"/>
-      <c r="L997" s="4"/>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D12" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D36" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D40" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="D41" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="D42" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="D44" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="D45" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="D46" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="D47" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="D48" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="D49" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="D50" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="D51" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="D52" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="D53" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="D54" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="D35" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D39" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D40" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D41" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D43" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D44" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D45" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D46" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="D47" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D48" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="D49" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="D50" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="D51" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="D52" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="D53" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId17"/>

</xml_diff>